<commit_message>
change clients import xlsx file format
</commit_message>
<xml_diff>
--- a/storage/app/public/excels/clients.xlsx
+++ b/storage/app/public/excels/clients.xlsx
@@ -1,30 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DMD-CHRISTIAN\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\satis-server\storage\app\public\excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{372735A2-71DE-486F-8E02-B9FFE1D5C4FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9525"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{68E47317-8F40-4CCC-A9A6-FE15F7F5F184}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>category_client</t>
+  </si>
+  <si>
+    <t>account_type</t>
+  </si>
+  <si>
+    <t>account_number</t>
+  </si>
   <si>
     <t>firstname</t>
   </si>
@@ -42,41 +59,14 @@
   </si>
   <si>
     <t>ville</t>
-  </si>
-  <si>
-    <t>institution</t>
-  </si>
-  <si>
-    <t>category_client</t>
-  </si>
-  <si>
-    <t>others_clients</t>
-  </si>
-  <si>
-    <t>other_identites</t>
-  </si>
-  <si>
-    <t>account_number</t>
-  </si>
-  <si>
-    <t>account_type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,10 +94,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -142,7 +130,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -154,7 +142,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -171,9 +159,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -201,14 +189,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -236,6 +241,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -387,77 +409,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42B4A72-DF77-47C2-894D-5011ED209F0B}">
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="45.85546875" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="26" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H3" s="2"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H4" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>